<commit_message>
add subject id from volumes file in the summary or final tables
</commit_message>
<xml_diff>
--- a/templates/volumes.xlsx
+++ b/templates/volumes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Treatment</t>
   </si>
@@ -37,13 +37,19 @@
   </si>
   <si>
     <t>ID*</t>
+  </si>
+  <si>
+    <t>Subject id</t>
+  </si>
+  <si>
+    <t>MU_001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +93,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="3">
@@ -157,7 +169,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -189,8 +201,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -213,8 +227,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -230,6 +247,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -245,6 +263,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -585,14 +604,15 @@
     <col min="1" max="1" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" spans="1:7" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -602,28 +622,34 @@
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <v>7101</v>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="6">
+        <v>7101</v>
+      </c>
       <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
change the template for volumes
</commit_message>
<xml_diff>
--- a/templates/volumes.xlsx
+++ b/templates/volumes.xlsx
@@ -115,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -123,51 +123,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -218,16 +173,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -596,7 +551,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -622,7 +577,7 @@
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -636,7 +591,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -645,7 +600,7 @@
       <c r="C2" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="8">
         <v>7101</v>
       </c>
       <c r="E2" s="4"/>

</xml_diff>